<commit_message>
Removed broken LFS image
</commit_message>
<xml_diff>
--- a/participants.xlsx
+++ b/participants.xlsx
@@ -441,59 +441,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Aman choudhary</t>
+          <t>Abhay Singh</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>gauravbadaliya420@gmail.com</t>
+          <t>abhaysinghktp800@gmail.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Badminton</t>
+          <t>Carrom Board</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>07988476183</t>
+          <t>09588014420</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>BCA</t>
+          <t>Faculty</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Abhay Singh</t>
+          <t>Aman choudhary</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>abhaysinghktp800@gmail.com</t>
+          <t>gauravbadaliya420@gmail.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Carrom Board</t>
+          <t>Badminton</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>09588014420</t>
+          <t>07988476183</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Faculty</t>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>BCA</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>BCA</t>
+          <t>BTECH</t>
         </is>
       </c>
     </row>

</xml_diff>